<commit_message>
Updating Validate_TimeScheduleRun workflow (Adding time frame to the dictionary)
</commit_message>
<xml_diff>
--- a/Data/Temp/Substitute Items - Template.xlsx
+++ b/Data/Temp/Substitute Items - Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V987917\Documents\UiPath\SubstituteItems_Performer\Data\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\700024\Documents\UiPath\Projects\UiPath\SubstituteItems_Performer\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE2993A-8F4C-49C5-B8D5-A1E2EC4B77AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9DDC8D-245B-4F1B-9835-58055E3B73C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{33062A72-EDEB-411B-BB95-26D606DC0DFF}"/>
+    <workbookView xWindow="5865" yWindow="6225" windowWidth="18315" windowHeight="13050" xr2:uid="{33062A72-EDEB-411B-BB95-26D606DC0DFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Substitute Items" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Buyer</t>
-  </si>
-  <si>
-    <t>SubItem</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
@@ -56,19 +44,7 @@
     <t>Created By:</t>
   </si>
   <si>
-    <t>MartBot</t>
-  </si>
-  <si>
-    <t>Substitution Code Previous</t>
-  </si>
-  <si>
-    <t>Substitution Code Final</t>
-  </si>
-  <si>
-    <t>Output Message</t>
-  </si>
-  <si>
-    <t>Status</t>
+    <t>UiPathBot</t>
   </si>
 </sst>
 </file>
@@ -78,16 +54,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,16 +112,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53EA421C-4AD6-47A2-B55D-A157262CBCDE}">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,132 +457,110 @@
     <col min="9" max="9" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4">
-        <f ca="1">TODAY()</f>
-        <v>45049</v>
-      </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B1" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45063</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1043,13 +986,6 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>